<commit_message>
Modification to not create new results.xlsx
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -353,7 +353,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -363,25 +363,9 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="n">
-        <v>1306.2</v>
+        <v>842.28</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="n">
-        <v>1310.48</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="n">
-        <v>1313.56</v>
-      </c>
-      <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>